<commit_message>
Mod in initial states
</commit_message>
<xml_diff>
--- a/Planner/GlobalAndEntrepreneurs/Graphs/Max_Omega.xlsx
+++ b/Planner/GlobalAndEntrepreneurs/Graphs/Max_Omega.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marya\Documents\GitHub\OptimalTaxation\Planner\GlobalAndEntrepreneurs\Graphs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariagon\Documents\OptimalTaxation\Planner\GlobalAndEntrepreneurs\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5903BF65-9EFF-42C0-AE73-388A515B23AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2159B44C-1B10-4288-919B-78CCDF6F47B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AEB8DBEC-5579-4831-977D-E01700606C00}"/>
+    <workbookView xWindow="-28920" yWindow="1215" windowWidth="29040" windowHeight="15840" xr2:uid="{AEB8DBEC-5579-4831-977D-E01700606C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>gp</t>
   </si>
@@ -52,8 +52,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -81,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -89,6 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,9 +126,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>102296</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>105819</xdr:rowOff>
+      <xdr:rowOff>74543</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -142,8 +151,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5838825" y="6378358"/>
-          <a:ext cx="3018642" cy="1164790"/>
+          <a:off x="5831791" y="6211344"/>
+          <a:ext cx="2933694" cy="1102199"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -812,11 +821,715 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>491205</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEB7B586-25C4-4496-B70E-36F7F9C54077}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10585174" y="381000"/>
+          <a:ext cx="2942857" cy="1190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>405491</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>37857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BE02DD7-7066-4152-B10A-F8229CEFDD34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14262652" y="381000"/>
+          <a:ext cx="2857143" cy="1942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>443586</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>18905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6EE06AA-A898-421C-982E-D8C93B3436E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10585174" y="2476500"/>
+          <a:ext cx="2895238" cy="1161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>291205</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7160D684-51DB-4B92-B796-3EDCE070C164}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14262652" y="2476500"/>
+          <a:ext cx="2742857" cy="2047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>538824</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52095944-BA7F-4896-BD8C-6D2556CE502D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10585174" y="4762500"/>
+          <a:ext cx="2990476" cy="1047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>386443</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50ABAC50-E4F9-4D85-BB00-B15581C73B94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14262652" y="4762500"/>
+          <a:ext cx="2838095" cy="1971429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>215348</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>33131</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>487505</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>80631</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6180EECB-F731-4C2A-92C1-2847AF52781E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10800522" y="7081631"/>
+          <a:ext cx="2723809" cy="1000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>434062</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>18810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E105DA3-0403-407B-9272-8A590E2E3B41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14262652" y="7048500"/>
+          <a:ext cx="2885714" cy="1923810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>173935</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>42703</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>17664</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A32A3EB8-8A06-4CBC-B463-26C820A9864D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10759109" y="9152283"/>
+          <a:ext cx="2933333" cy="1152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>367396</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>66429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A75EDD9-AF4A-4828-A445-101AFAE50415}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14262652" y="9144000"/>
+          <a:ext cx="2819048" cy="1971429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>500729</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>114167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D0A1589-7B91-4792-8471-A992DD9EF414}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10585174" y="11239500"/>
+          <a:ext cx="2952381" cy="1066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>348348</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>37857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC66D96D-9322-471A-9FF5-7D4FE9241694}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14262652" y="11239500"/>
+          <a:ext cx="2800000" cy="1942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>472157</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAD122EE-825D-4500-8DC7-A5D2D60FF051}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19778870" y="381000"/>
+          <a:ext cx="2923809" cy="1142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>224538</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>37857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97696043-F75C-4CB0-AA79-F8E3EB8EAFC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22843435" y="381000"/>
+          <a:ext cx="2676190" cy="1942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>395967</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{331DC2C5-AF09-49B6-A3FD-6350A724B1DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19778870" y="2667000"/>
+          <a:ext cx="2847619" cy="1190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>415015</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1A3BEB4-A8BB-4782-B89C-248D9ED1A8DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22843435" y="2667000"/>
+          <a:ext cx="2866667" cy="2009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1112,18 +1825,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE778A9-4D3C-48C5-AB4C-FA27ECD4C5EC}">
-  <dimension ref="B2:N68"/>
+  <dimension ref="B2:AF68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AL15" sqref="AL15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1147,8 +1860,17 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
+      <c r="O2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0.99</v>
       </c>
@@ -1158,8 +1880,26 @@
       <c r="D3">
         <v>1.349</v>
       </c>
+      <c r="O3">
+        <v>0.98</v>
+      </c>
+      <c r="P3">
+        <v>9.7704890686249204</v>
+      </c>
+      <c r="Q3">
+        <v>1.339</v>
+      </c>
+      <c r="AD3">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="AE3">
+        <v>9.6998061850476596</v>
+      </c>
+      <c r="AF3">
+        <v>1.343</v>
+      </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.97</v>
       </c>
@@ -1170,7 +1910,30 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="P14">
+        <v>9.6839753411006502</v>
+      </c>
+      <c r="Q14">
+        <v>1.3440000000000001</v>
+      </c>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AD15">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="AE15">
+        <v>9.6998061850476596</v>
+      </c>
+      <c r="AF15">
+        <v>1.343</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.95</v>
       </c>
@@ -1181,7 +1944,18 @@
         <v>1.3129999999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="P26">
+        <v>9.6565756783133896</v>
+      </c>
+      <c r="Q26">
+        <v>1.347</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>0.9</v>
       </c>
@@ -1192,7 +1966,18 @@
         <v>1.272054</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="P38">
+        <v>9.6632421391671102</v>
+      </c>
+      <c r="Q38">
+        <v>1.3480000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.8</v>
       </c>
@@ -1203,7 +1988,18 @@
         <v>1.1910000000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>0.98950000000000005</v>
+      </c>
+      <c r="P49">
+        <v>9.8359765818973095</v>
+      </c>
+      <c r="Q49">
+        <v>1.3480000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>0.7</v>
       </c>
@@ -1214,7 +2010,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>0.6</v>
       </c>
@@ -1223,6 +2019,17 @@
       </c>
       <c r="D58">
         <v>1.0269999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <v>0.9899</v>
+      </c>
+      <c r="P60">
+        <v>9.6348250887122902</v>
+      </c>
+      <c r="Q60">
+        <v>1.349</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
@@ -1242,6 +2049,7 @@
     <mergeCell ref="E2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change par and propositions.
</commit_message>
<xml_diff>
--- a/Planner/GlobalAndEntrepreneurs/Graphs/Max_Omega.xlsx
+++ b/Planner/GlobalAndEntrepreneurs/Graphs/Max_Omega.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariagon\Documents\OptimalTaxation\Planner\GlobalAndEntrepreneurs\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2159B44C-1B10-4288-919B-78CCDF6F47B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C573E588-86C6-4FC3-954F-820801326A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1215" windowWidth="29040" windowHeight="15840" xr2:uid="{AEB8DBEC-5579-4831-977D-E01700606C00}"/>
+    <workbookView xWindow="-28920" yWindow="1215" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AEB8DBEC-5579-4831-977D-E01700606C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mod h" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>gp</t>
   </si>
@@ -46,6 +47,51 @@
   </si>
   <si>
     <t>e(θ_w)_lb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    gp     =   0.983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ue0    =   100.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ue0    =   630.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    μe0    =   0.0 - 1.0e-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ye0    =   0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    λe0    =   1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    le0    =   0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ωe0    =   0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ωe0    =   1.34232</t>
+  </si>
+  <si>
+    <t>El del equilibrio!</t>
+  </si>
+  <si>
+    <t>Equilibrium in new scenary:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    gp     =   0.989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    #ue0    =   100.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ue0    =   585.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ωe0    =   1.3</t>
   </si>
 </sst>
 </file>
@@ -69,12 +115,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,15 +141,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,7 +179,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>74543</xdr:rowOff>
     </xdr:to>
@@ -170,9 +223,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>183061</xdr:colOff>
+      <xdr:colOff>177346</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>32490</xdr:rowOff>
+      <xdr:rowOff>26775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -214,9 +267,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>47258</xdr:colOff>
+      <xdr:colOff>54878</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>9367</xdr:rowOff>
+      <xdr:rowOff>16987</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -260,7 +313,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>85758</xdr:rowOff>
+      <xdr:rowOff>95283</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -302,9 +355,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>66323</xdr:colOff>
+      <xdr:colOff>56798</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>66526</xdr:rowOff>
+      <xdr:rowOff>57001</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -346,9 +399,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
+      <xdr:colOff>93344</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>49800</xdr:rowOff>
+      <xdr:rowOff>53610</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -390,7 +443,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>561063</xdr:colOff>
+      <xdr:colOff>551538</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>155615</xdr:rowOff>
     </xdr:to>
@@ -436,7 +489,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>37360</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>124069</xdr:rowOff>
+      <xdr:rowOff>133594</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -478,9 +531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>287055</xdr:colOff>
+      <xdr:colOff>283245</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>158388</xdr:rowOff>
+      <xdr:rowOff>164103</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -522,7 +575,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>180359</xdr:colOff>
+      <xdr:colOff>170834</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>34333</xdr:rowOff>
     </xdr:to>
@@ -566,7 +619,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>126598</xdr:colOff>
+      <xdr:colOff>130408</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>112447</xdr:rowOff>
     </xdr:to>
@@ -610,9 +663,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>138598</xdr:colOff>
+      <xdr:colOff>134788</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>46160</xdr:rowOff>
+      <xdr:rowOff>53780</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -654,9 +707,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>391691</xdr:colOff>
+      <xdr:colOff>401216</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>130478</xdr:rowOff>
+      <xdr:rowOff>134288</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -698,9 +751,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>143528</xdr:colOff>
+      <xdr:colOff>135908</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>61979</xdr:rowOff>
+      <xdr:rowOff>58169</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -742,9 +795,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>141743</xdr:colOff>
+      <xdr:colOff>132218</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>88071</xdr:rowOff>
+      <xdr:rowOff>91881</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -786,9 +839,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>352295</xdr:colOff>
+      <xdr:colOff>359915</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>108401</xdr:rowOff>
+      <xdr:rowOff>102686</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -830,9 +883,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>491205</xdr:colOff>
+      <xdr:colOff>485490</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>47476</xdr:rowOff>
+      <xdr:rowOff>55096</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -874,7 +927,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>405491</xdr:colOff>
+      <xdr:colOff>401681</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>37857</xdr:rowOff>
     </xdr:to>
@@ -918,9 +971,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>443586</xdr:colOff>
+      <xdr:colOff>439776</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>18905</xdr:rowOff>
+      <xdr:rowOff>22715</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -962,9 +1015,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>291205</xdr:colOff>
+      <xdr:colOff>287395</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>142619</xdr:rowOff>
+      <xdr:rowOff>133094</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1006,9 +1059,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>538824</xdr:colOff>
+      <xdr:colOff>544539</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>95119</xdr:rowOff>
+      <xdr:rowOff>98929</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1050,9 +1103,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>386443</xdr:colOff>
+      <xdr:colOff>392158</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>66429</xdr:rowOff>
+      <xdr:rowOff>56904</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1094,9 +1147,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>487505</xdr:colOff>
+      <xdr:colOff>479885</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>80631</xdr:rowOff>
+      <xdr:rowOff>86346</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1138,9 +1191,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>434062</xdr:colOff>
+      <xdr:colOff>437872</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>18810</xdr:rowOff>
+      <xdr:rowOff>22620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1182,9 +1235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>42703</xdr:colOff>
+      <xdr:colOff>48418</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>17664</xdr:rowOff>
+      <xdr:rowOff>21474</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1226,9 +1279,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>367396</xdr:colOff>
+      <xdr:colOff>363586</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>66429</xdr:rowOff>
+      <xdr:rowOff>56904</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1270,7 +1323,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>500729</xdr:colOff>
+      <xdr:colOff>506444</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>114167</xdr:rowOff>
     </xdr:to>
@@ -1314,7 +1367,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>348348</xdr:colOff>
+      <xdr:colOff>354063</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>37857</xdr:rowOff>
     </xdr:to>
@@ -1358,9 +1411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>472157</xdr:colOff>
+      <xdr:colOff>475967</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>190357</xdr:rowOff>
+      <xdr:rowOff>175117</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1402,7 +1455,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>224538</xdr:colOff>
+      <xdr:colOff>218823</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>37857</xdr:rowOff>
     </xdr:to>
@@ -1446,9 +1499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>395967</xdr:colOff>
+      <xdr:colOff>399777</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>47476</xdr:rowOff>
+      <xdr:rowOff>55096</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1490,9 +1543,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>415015</xdr:colOff>
+      <xdr:colOff>409300</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>104524</xdr:rowOff>
+      <xdr:rowOff>94999</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1517,6 +1570,99 @@
         <a:xfrm>
           <a:off x="22843435" y="2667000"/>
           <a:ext cx="2866667" cy="2009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>456838</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{248A6480-FC11-4FF4-970C-B07206AEA6BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514600" y="542925"/>
+          <a:ext cx="2895238" cy="1152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>466362</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152155</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C20A64E-4036-4E81-BC45-FB2DC4F5F1FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6172200" y="542925"/>
+          <a:ext cx="2904762" cy="1961905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1825,18 +1971,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE778A9-4D3C-48C5-AB4C-FA27ECD4C5EC}">
-  <dimension ref="B2:AF68"/>
+  <dimension ref="B2:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AL15" sqref="AL15"/>
+    <sheetView topLeftCell="AC13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD29" sqref="AD29:AF34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1846,20 +1993,20 @@
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
       <c r="O2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1870,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0.99</v>
       </c>
@@ -1899,7 +2046,7 @@
         <v>1.343</v>
       </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0.97</v>
       </c>
@@ -1910,7 +2057,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.3">
       <c r="O14">
         <v>0.98499999999999999</v>
       </c>
@@ -1920,9 +2067,9 @@
       <c r="Q14">
         <v>1.3440000000000001</v>
       </c>
-      <c r="R14" s="3"/>
-    </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
       <c r="AD15">
         <v>0.98299999999999998</v>
       </c>
@@ -1933,7 +2080,7 @@
         <v>1.343</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0.95</v>
       </c>
@@ -1944,7 +2091,7 @@
         <v>1.3129999999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.3">
       <c r="O26">
         <v>0.98799999999999999</v>
       </c>
@@ -1954,8 +2101,55 @@
       <c r="Q26">
         <v>1.347</v>
       </c>
-    </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AD26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE26" s="4"/>
+      <c r="AG26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+    </row>
+    <row r="28" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AD28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE28" s="4"/>
+    </row>
+    <row r="29" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AD29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE29" s="4"/>
+    </row>
+    <row r="30" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AD30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE30" s="4"/>
+    </row>
+    <row r="31" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AD31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE31" s="4"/>
+    </row>
+    <row r="32" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AD32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE32" s="4"/>
+    </row>
+    <row r="33" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AD33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE33" s="4"/>
+    </row>
+    <row r="34" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>0.9</v>
       </c>
@@ -1965,8 +2159,18 @@
       <c r="D34" s="1">
         <v>1.272054</v>
       </c>
-    </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AD34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE34" s="4"/>
+    </row>
+    <row r="35" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AD35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE35" s="4"/>
+    </row>
+    <row r="38" spans="2:31" x14ac:dyDescent="0.3">
       <c r="O38">
         <v>0.98899999999999999</v>
       </c>
@@ -1977,7 +2181,7 @@
         <v>1.3480000000000001</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>0.8</v>
       </c>
@@ -1988,7 +2192,7 @@
         <v>1.1910000000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.3">
       <c r="O49">
         <v>0.98950000000000005</v>
       </c>
@@ -1999,7 +2203,7 @@
         <v>1.3480000000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>0.7</v>
       </c>
@@ -2010,7 +2214,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>0.6</v>
       </c>
@@ -2021,7 +2225,7 @@
         <v>1.0269999999999999</v>
       </c>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.3">
       <c r="O60">
         <v>0.9899</v>
       </c>
@@ -2032,7 +2236,7 @@
         <v>1.349</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68">
         <v>0.5</v>
       </c>
@@ -2052,4 +2256,73 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C1D396-AA44-45C4-81D2-BCFA990AD9AC}">
+  <dimension ref="B2:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>